<commit_message>
update matches for SPE_489
</commit_message>
<xml_diff>
--- a/CD-valid/Input/Metadatatps.xlsx
+++ b/CD-valid/Input/Metadatatps.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhabiby\Documents\GitHub\eu-data-validation\CD-valid\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C775C109-2E66-462E-95D8-A91631E81B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0A9088-273C-423C-9B85-49C9A7FEC99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$85</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="395">
   <si>
     <t>GPP_Variable_Name</t>
   </si>
@@ -700,12 +716,6 @@
     <t>JSE_affordcosts</t>
   </si>
   <si>
-    <t>SPE_489_qa5_2</t>
-  </si>
-  <si>
-    <t>Q5_2. How important for you personally are the following points? (2) Court proceedings are not excessively long or costly</t>
-  </si>
-  <si>
     <t>7.3: Civil justice is people-centered, accessible, efficient, and outcome-oriented</t>
   </si>
   <si>
@@ -846,12 +856,6 @@
     <t>LEP_indprosecutors</t>
   </si>
   <si>
-    <t>SPE_489_qa5_4</t>
-  </si>
-  <si>
-    <t>Q5_4. How important for you personally are the following points? (4) The police and prosecution service investigate crimes properly including those committed by politicians or influential persons and they are not under the influence of politicians or economic interests</t>
-  </si>
-  <si>
     <t>8.2: Prosecution and pre-trial process</t>
   </si>
   <si>
@@ -1090,12 +1094,6 @@
     <t>ROL_constprotection_imp</t>
   </si>
   <si>
-    <t>SPE_489_qa5_1</t>
-  </si>
-  <si>
-    <t>Q5_1. How important for you personally are the following points? (1) If your rights are not respected, you can have them upheld by an independent court</t>
-  </si>
-  <si>
     <t>q59e</t>
   </si>
   <si>
@@ -1238,6 +1236,15 @@
   </si>
   <si>
     <t>EU_Questionnaire</t>
+  </si>
+  <si>
+    <t>NUTS Level</t>
+  </si>
+  <si>
+    <t>Q6_2. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (2) Court proceedings are not excessively long or costly</t>
+  </si>
+  <si>
+    <t>SPE_489_qa6_2</t>
   </si>
 </sst>
 </file>
@@ -1596,15 +1603,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M85"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1639,13 +1652,16 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1685,8 +1701,11 @@
       <c r="M2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1726,8 +1745,11 @@
       <c r="M3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1767,8 +1789,11 @@
       <c r="M4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1808,8 +1833,11 @@
       <c r="M5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1849,8 +1877,11 @@
       <c r="M6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1890,8 +1921,11 @@
       <c r="M7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1931,8 +1965,11 @@
       <c r="M8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1972,8 +2009,11 @@
       <c r="M9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -2013,8 +2053,11 @@
       <c r="M10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -2054,8 +2097,11 @@
       <c r="M11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -2095,8 +2141,11 @@
       <c r="M12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -2136,8 +2185,11 @@
       <c r="M13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -2177,8 +2229,11 @@
       <c r="M14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -2218,8 +2273,11 @@
       <c r="M15" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -2259,8 +2317,11 @@
       <c r="M16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -2300,8 +2361,11 @@
       <c r="M17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2341,8 +2405,11 @@
       <c r="M18" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -2382,8 +2449,11 @@
       <c r="M19" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -2423,8 +2493,11 @@
       <c r="M20" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -2464,8 +2537,11 @@
       <c r="M21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -2505,8 +2581,11 @@
       <c r="M22" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -2546,8 +2625,11 @@
       <c r="M23" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -2587,8 +2669,11 @@
       <c r="M24" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -2628,8 +2713,11 @@
       <c r="M25" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>130</v>
       </c>
@@ -2669,8 +2757,11 @@
       <c r="M26" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -2710,8 +2801,11 @@
       <c r="M27" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>143</v>
       </c>
@@ -2751,8 +2845,11 @@
       <c r="M28" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -2792,8 +2889,11 @@
       <c r="M29" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -2833,8 +2933,11 @@
       <c r="M30" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -2874,8 +2977,11 @@
       <c r="M31" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2915,8 +3021,11 @@
       <c r="M32" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -2956,8 +3065,11 @@
       <c r="M33" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -2997,8 +3109,11 @@
       <c r="M34" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -3038,8 +3153,11 @@
       <c r="M35" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -3074,13 +3192,16 @@
         <v>22</v>
       </c>
       <c r="L36" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="M36" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>168</v>
       </c>
@@ -3115,13 +3236,16 @@
         <v>41</v>
       </c>
       <c r="L37" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="M37" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -3156,13 +3280,16 @@
         <v>41</v>
       </c>
       <c r="L38" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="M38" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>176</v>
       </c>
@@ -3202,8 +3329,11 @@
       <c r="M39" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>180</v>
       </c>
@@ -3243,8 +3373,11 @@
       <c r="M40" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -3284,8 +3417,11 @@
       <c r="M41" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>191</v>
       </c>
@@ -3325,8 +3461,11 @@
       <c r="M42" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -3366,8 +3505,11 @@
       <c r="M43" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -3407,8 +3549,11 @@
       <c r="M44" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>206</v>
       </c>
@@ -3448,8 +3593,11 @@
       <c r="M45" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>211</v>
       </c>
@@ -3489,8 +3637,11 @@
       <c r="M46" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>211</v>
       </c>
@@ -3530,13 +3681,16 @@
       <c r="M47" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>219</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>394</v>
       </c>
       <c r="C48" t="s">
         <v>132</v>
@@ -3545,13 +3699,13 @@
         <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>221</v>
+        <v>393</v>
       </c>
       <c r="F48" t="s">
         <v>82</v>
       </c>
       <c r="G48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H48" t="s">
         <v>19</v>
@@ -3566,18 +3720,21 @@
         <v>41</v>
       </c>
       <c r="L48" t="s">
+        <v>221</v>
+      </c>
+      <c r="M48" t="s">
+        <v>222</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>223</v>
       </c>
-      <c r="M48" t="s">
+      <c r="B49" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>225</v>
-      </c>
-      <c r="B49" t="s">
-        <v>226</v>
       </c>
       <c r="C49" t="s">
         <v>132</v>
@@ -3586,13 +3743,13 @@
         <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F49" t="s">
         <v>82</v>
       </c>
       <c r="G49" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H49" t="s">
         <v>19</v>
@@ -3607,18 +3764,21 @@
         <v>41</v>
       </c>
       <c r="L49" t="s">
+        <v>227</v>
+      </c>
+      <c r="M49" t="s">
+        <v>228</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>229</v>
       </c>
-      <c r="M49" t="s">
+      <c r="B50" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>231</v>
-      </c>
-      <c r="B50" t="s">
-        <v>232</v>
       </c>
       <c r="C50" t="s">
         <v>109</v>
@@ -3627,7 +3787,7 @@
         <v>110</v>
       </c>
       <c r="E50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F50" t="s">
         <v>45</v>
@@ -3648,18 +3808,21 @@
         <v>41</v>
       </c>
       <c r="L50" t="s">
+        <v>232</v>
+      </c>
+      <c r="M50" t="s">
+        <v>233</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>234</v>
       </c>
-      <c r="M50" t="s">
+      <c r="B51" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>236</v>
-      </c>
-      <c r="B51" t="s">
-        <v>237</v>
       </c>
       <c r="C51" t="s">
         <v>132</v>
@@ -3668,13 +3831,13 @@
         <v>52</v>
       </c>
       <c r="E51" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F51" t="s">
         <v>98</v>
       </c>
       <c r="G51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H51" t="s">
         <v>19</v>
@@ -3689,18 +3852,21 @@
         <v>41</v>
       </c>
       <c r="L51" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M51" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C52" t="s">
         <v>132</v>
@@ -3709,7 +3875,7 @@
         <v>52</v>
       </c>
       <c r="E52" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F52" t="s">
         <v>36</v>
@@ -3730,18 +3896,21 @@
         <v>41</v>
       </c>
       <c r="L52" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M52" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B53" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C53" t="s">
         <v>132</v>
@@ -3750,7 +3919,7 @@
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F53" t="s">
         <v>82</v>
@@ -3771,18 +3940,21 @@
         <v>41</v>
       </c>
       <c r="L53" t="s">
+        <v>238</v>
+      </c>
+      <c r="M53" t="s">
+        <v>239</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>234</v>
+      </c>
+      <c r="B54" t="s">
         <v>240</v>
-      </c>
-      <c r="M53" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>236</v>
-      </c>
-      <c r="B54" t="s">
-        <v>242</v>
       </c>
       <c r="C54" t="s">
         <v>34</v>
@@ -3791,13 +3963,13 @@
         <v>15</v>
       </c>
       <c r="E54" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F54" t="s">
         <v>98</v>
       </c>
       <c r="G54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H54" t="s">
         <v>38</v>
@@ -3812,18 +3984,21 @@
         <v>41</v>
       </c>
       <c r="L54" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M54" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B55" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C55" t="s">
         <v>59</v>
@@ -3832,13 +4007,13 @@
         <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F55" t="s">
         <v>98</v>
       </c>
       <c r="G55" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H55" t="s">
         <v>38</v>
@@ -3853,18 +4028,21 @@
         <v>41</v>
       </c>
       <c r="L55" t="s">
+        <v>245</v>
+      </c>
+      <c r="M55" t="s">
+        <v>246</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>247</v>
       </c>
-      <c r="M55" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>249</v>
-      </c>
       <c r="B56" t="s">
-        <v>220</v>
+        <v>394</v>
       </c>
       <c r="C56" t="s">
         <v>132</v>
@@ -3873,13 +4051,13 @@
         <v>52</v>
       </c>
       <c r="E56" t="s">
-        <v>221</v>
+        <v>393</v>
       </c>
       <c r="F56" t="s">
         <v>82</v>
       </c>
       <c r="G56" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H56" t="s">
         <v>19</v>
@@ -3894,15 +4072,18 @@
         <v>41</v>
       </c>
       <c r="L56" t="s">
+        <v>248</v>
+      </c>
+      <c r="M56" t="s">
+        <v>249</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>250</v>
-      </c>
-      <c r="M56" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>252</v>
       </c>
       <c r="B57" t="s">
         <v>197</v>
@@ -3920,7 +4101,7 @@
         <v>82</v>
       </c>
       <c r="G57" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H57" t="s">
         <v>19</v>
@@ -3935,18 +4116,21 @@
         <v>41</v>
       </c>
       <c r="L57" t="s">
+        <v>252</v>
+      </c>
+      <c r="M57" t="s">
+        <v>253</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>254</v>
       </c>
-      <c r="M57" t="s">
+      <c r="B58" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>256</v>
-      </c>
-      <c r="B58" t="s">
-        <v>257</v>
       </c>
       <c r="C58" t="s">
         <v>27</v>
@@ -3955,13 +4139,13 @@
         <v>28</v>
       </c>
       <c r="E58" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F58" t="s">
         <v>98</v>
       </c>
       <c r="G58" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H58" t="s">
         <v>19</v>
@@ -3976,18 +4160,21 @@
         <v>41</v>
       </c>
       <c r="L58" t="s">
+        <v>258</v>
+      </c>
+      <c r="M58" t="s">
+        <v>259</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>260</v>
       </c>
-      <c r="M58" t="s">
+      <c r="B59" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>262</v>
-      </c>
-      <c r="B59" t="s">
-        <v>263</v>
       </c>
       <c r="C59" t="s">
         <v>132</v>
@@ -3996,7 +4183,7 @@
         <v>52</v>
       </c>
       <c r="E59" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F59" t="s">
         <v>36</v>
@@ -4017,18 +4204,21 @@
         <v>41</v>
       </c>
       <c r="L59" t="s">
+        <v>263</v>
+      </c>
+      <c r="M59" t="s">
+        <v>264</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>265</v>
       </c>
-      <c r="M59" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>267</v>
-      </c>
       <c r="B60" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
         <v>132</v>
@@ -4037,13 +4227,13 @@
         <v>52</v>
       </c>
       <c r="E60" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F60" t="s">
         <v>36</v>
       </c>
       <c r="G60" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="H60" t="s">
         <v>19</v>
@@ -4058,18 +4248,21 @@
         <v>41</v>
       </c>
       <c r="L60" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="M60" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B61" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -4078,7 +4271,7 @@
         <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F61" t="s">
         <v>17</v>
@@ -4099,18 +4292,21 @@
         <v>22</v>
       </c>
       <c r="L61" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="M61" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B62" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -4119,13 +4315,13 @@
         <v>15</v>
       </c>
       <c r="E62" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F62" t="s">
         <v>98</v>
       </c>
       <c r="G62" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H62" t="s">
         <v>19</v>
@@ -4140,18 +4336,21 @@
         <v>41</v>
       </c>
       <c r="L62" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="M62" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C63" t="s">
         <v>34</v>
@@ -4160,7 +4359,7 @@
         <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F63" t="s">
         <v>17</v>
@@ -4181,18 +4380,21 @@
         <v>41</v>
       </c>
       <c r="L63" t="s">
+        <v>278</v>
+      </c>
+      <c r="M63" t="s">
+        <v>279</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>282</v>
       </c>
-      <c r="M63" t="s">
+      <c r="B64" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>286</v>
-      </c>
-      <c r="B64" t="s">
-        <v>287</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
@@ -4201,13 +4403,13 @@
         <v>15</v>
       </c>
       <c r="E64" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F64" t="s">
         <v>98</v>
       </c>
       <c r="G64" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H64" t="s">
         <v>19</v>
@@ -4222,18 +4424,21 @@
         <v>41</v>
       </c>
       <c r="L64" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="M64" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B65" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C65" t="s">
         <v>14</v>
@@ -4242,13 +4447,13 @@
         <v>15</v>
       </c>
       <c r="E65" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F65" t="s">
         <v>17</v>
       </c>
       <c r="G65" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H65" t="s">
         <v>19</v>
@@ -4263,18 +4468,21 @@
         <v>22</v>
       </c>
       <c r="L65" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="M65" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B66" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C66" t="s">
         <v>59</v>
@@ -4283,13 +4491,13 @@
         <v>15</v>
       </c>
       <c r="E66" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F66" t="s">
         <v>98</v>
       </c>
       <c r="G66" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H66" t="s">
         <v>38</v>
@@ -4304,18 +4512,21 @@
         <v>22</v>
       </c>
       <c r="L66" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="M66" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B67" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C67" t="s">
         <v>59</v>
@@ -4324,13 +4535,13 @@
         <v>15</v>
       </c>
       <c r="E67" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F67" t="s">
         <v>98</v>
       </c>
       <c r="G67" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H67" t="s">
         <v>38</v>
@@ -4345,18 +4556,21 @@
         <v>22</v>
       </c>
       <c r="L67" t="s">
+        <v>297</v>
+      </c>
+      <c r="M67" t="s">
+        <v>298</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>301</v>
       </c>
-      <c r="M67" t="s">
+      <c r="B68" t="s">
         <v>302</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>305</v>
-      </c>
-      <c r="B68" t="s">
-        <v>306</v>
       </c>
       <c r="C68" t="s">
         <v>59</v>
@@ -4365,13 +4579,13 @@
         <v>15</v>
       </c>
       <c r="E68" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F68" t="s">
         <v>98</v>
       </c>
       <c r="G68" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H68" t="s">
         <v>38</v>
@@ -4386,18 +4600,21 @@
         <v>22</v>
       </c>
       <c r="L68" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="M68" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B69" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C69" t="s">
         <v>59</v>
@@ -4406,13 +4623,13 @@
         <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F69" t="s">
         <v>98</v>
       </c>
       <c r="G69" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H69" t="s">
         <v>38</v>
@@ -4427,18 +4644,21 @@
         <v>22</v>
       </c>
       <c r="L69" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="M69" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B70" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C70" t="s">
         <v>125</v>
@@ -4447,13 +4667,13 @@
         <v>28</v>
       </c>
       <c r="E70" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F70" t="s">
         <v>98</v>
       </c>
       <c r="G70" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H70" t="s">
         <v>19</v>
@@ -4468,18 +4688,21 @@
         <v>22</v>
       </c>
       <c r="L70" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="M70" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="N70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B71" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C71" t="s">
         <v>125</v>
@@ -4488,13 +4711,13 @@
         <v>28</v>
       </c>
       <c r="E71" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F71" t="s">
         <v>98</v>
       </c>
       <c r="G71" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H71" t="s">
         <v>19</v>
@@ -4509,18 +4732,21 @@
         <v>22</v>
       </c>
       <c r="L71" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M71" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+      <c r="N71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B72" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C72" t="s">
         <v>59</v>
@@ -4529,13 +4755,13 @@
         <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F72" t="s">
         <v>98</v>
       </c>
       <c r="G72" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H72" t="s">
         <v>38</v>
@@ -4550,15 +4776,18 @@
         <v>22</v>
       </c>
       <c r="L72" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="M72" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+        <v>328</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B73" t="s">
         <v>136</v>
@@ -4576,7 +4805,7 @@
         <v>98</v>
       </c>
       <c r="G73" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H73" t="s">
         <v>38</v>
@@ -4591,18 +4820,21 @@
         <v>22</v>
       </c>
       <c r="L73" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="M73" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B74" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C74" t="s">
         <v>59</v>
@@ -4611,13 +4843,13 @@
         <v>15</v>
       </c>
       <c r="E74" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F74" t="s">
         <v>98</v>
       </c>
       <c r="G74" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H74" t="s">
         <v>38</v>
@@ -4632,18 +4864,21 @@
         <v>22</v>
       </c>
       <c r="L74" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="M74" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B75" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C75" t="s">
         <v>132</v>
@@ -4652,13 +4887,13 @@
         <v>52</v>
       </c>
       <c r="E75" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F75" t="s">
         <v>17</v>
       </c>
       <c r="G75" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H75" t="s">
         <v>19</v>
@@ -4667,24 +4902,27 @@
         <v>20</v>
       </c>
       <c r="J75" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K75" t="s">
         <v>22</v>
       </c>
       <c r="L75" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="M75" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+      <c r="N75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B76" t="s">
-        <v>348</v>
+        <v>224</v>
       </c>
       <c r="C76" t="s">
         <v>132</v>
@@ -4693,7 +4931,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="s">
-        <v>349</v>
+        <v>225</v>
       </c>
       <c r="F76" t="s">
         <v>45</v>
@@ -4708,24 +4946,27 @@
         <v>20</v>
       </c>
       <c r="J76" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K76" t="s">
         <v>22</v>
       </c>
       <c r="L76" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="M76" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+        <v>345</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B77" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C77" t="s">
         <v>132</v>
@@ -4734,13 +4975,13 @@
         <v>52</v>
       </c>
       <c r="E77" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="F77" t="s">
         <v>98</v>
       </c>
       <c r="G77" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="H77" t="s">
         <v>19</v>
@@ -4749,24 +4990,27 @@
         <v>20</v>
       </c>
       <c r="J77" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K77" t="s">
         <v>22</v>
       </c>
       <c r="L77" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="M77" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+        <v>351</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B78" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C78" t="s">
         <v>132</v>
@@ -4775,13 +5019,13 @@
         <v>52</v>
       </c>
       <c r="E78" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F78" t="s">
         <v>98</v>
       </c>
       <c r="G78" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H78" t="s">
         <v>19</v>
@@ -4790,24 +5034,27 @@
         <v>20</v>
       </c>
       <c r="J78" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K78" t="s">
         <v>22</v>
       </c>
       <c r="L78" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="M78" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+        <v>356</v>
+      </c>
+      <c r="N78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B79" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C79" t="s">
         <v>34</v>
@@ -4816,7 +5063,7 @@
         <v>15</v>
       </c>
       <c r="E79" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F79" t="s">
         <v>45</v>
@@ -4831,24 +5078,27 @@
         <v>30</v>
       </c>
       <c r="J79" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K79" t="s">
         <v>22</v>
       </c>
       <c r="L79" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="M79" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+        <v>361</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B80" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C80" t="s">
         <v>132</v>
@@ -4857,7 +5107,7 @@
         <v>52</v>
       </c>
       <c r="E80" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F80" t="s">
         <v>45</v>
@@ -4872,24 +5122,27 @@
         <v>20</v>
       </c>
       <c r="J80" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K80" t="s">
         <v>22</v>
       </c>
       <c r="L80" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="M80" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+        <v>361</v>
+      </c>
+      <c r="N80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B81" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C81" t="s">
         <v>34</v>
@@ -4898,7 +5151,7 @@
         <v>15</v>
       </c>
       <c r="E81" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F81" t="s">
         <v>45</v>
@@ -4919,33 +5172,36 @@
         <v>41</v>
       </c>
       <c r="L81" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="M81" t="s">
+        <v>361</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>366</v>
+      </c>
+      <c r="B82" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>372</v>
-      </c>
-      <c r="B82" t="s">
-        <v>373</v>
-      </c>
       <c r="C82" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D82" t="s">
         <v>28</v>
       </c>
       <c r="E82" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="F82" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G82" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H82" t="s">
         <v>19</v>
@@ -4960,18 +5216,21 @@
         <v>22</v>
       </c>
       <c r="L82" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="M82" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+        <v>373</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B83" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
@@ -4980,7 +5239,7 @@
         <v>110</v>
       </c>
       <c r="E83" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="F83" t="s">
         <v>112</v>
@@ -5001,18 +5260,21 @@
         <v>41</v>
       </c>
       <c r="L83" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="M83" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+        <v>378</v>
+      </c>
+      <c r="N83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B84" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
@@ -5021,7 +5283,7 @@
         <v>110</v>
       </c>
       <c r="E84" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="F84" t="s">
         <v>112</v>
@@ -5042,18 +5304,21 @@
         <v>41</v>
       </c>
       <c r="L84" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="M84" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+      <c r="N84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B85" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
@@ -5062,7 +5327,7 @@
         <v>110</v>
       </c>
       <c r="E85" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F85" t="s">
         <v>112</v>
@@ -5083,21 +5348,42 @@
         <v>41</v>
       </c>
       <c r="L85" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="M85" t="s">
-        <v>394</v>
+        <v>388</v>
+      </c>
+      <c r="N85">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N85" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1e7d1cb27deb8d263e2d401018ecc8eb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b7905617efe2037a5881c093ccc8f66d" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
     <xsd:import namespace="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
     <xsd:element name="properties">
@@ -5132,7 +5418,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="69276225-f05c-44c5-92dc-c999460a4149" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -5151,7 +5437,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -5183,7 +5469,7 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c40d4899-0986-466d-9443-4d7b8518a0f2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c40d4899-0986-466d-9443-4d7b8518a0f2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -5254,8 +5540,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -5344,7 +5630,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5354,9 +5640,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8872F2AE-4B15-4C68-B863-D8D1701B4494}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E3882BF-B03B-4509-9C72-07D9FC477D3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA95542-0BB8-4523-B4C4-2E72CF4D462C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{015D247E-FAB5-4D14-9F04-7B9489115DA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA95542-0BB8-4523-B4C4-2E72CF4D462C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>